<commit_message>
Amélioration du SEO + Accessibilité
Amélioration du SEO + Accessibilité
Ajout d'erreurs d'accessibilité à l'audit.
</commit_message>
<xml_diff>
--- a/ressources/Modèle-audit-SEO.xlsx
+++ b/ressources/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="75">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -46,24 +46,27 @@
     <t xml:space="preserve">Référence</t>
   </si>
   <si>
+    <t xml:space="preserve">SEO + Accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langue du document non spécifiée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">html lang est configuré sur « Default »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spécifier la langue du document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page2.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO</t>
   </si>
   <si>
-    <t xml:space="preserve">index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Langue du document non spécifiée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">html lang est configuré sur « Default »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spécifier la langue du document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">page2.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">Balise keywords invalide</t>
   </si>
   <si>
@@ -130,9 +133,6 @@
     <t xml:space="preserve">Utiliser un nom significatif</t>
   </si>
   <si>
-    <t xml:space="preserve">SEO + Accessibilité</t>
-  </si>
-  <si>
     <t xml:space="preserve">Texte superflu pour augmenter le référencement</t>
   </si>
   <si>
@@ -212,6 +212,39 @@
   </si>
   <si>
     <t xml:space="preserve">Remplacer par du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lien vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La balise de lien ne contient rien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insérer du texte identifiant le lien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 fois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contraste faible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contraste entre le texte et le fond est trop faible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer de couleurs avec un contraste plus élevé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 fois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas d’attribut for pour la balise label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La balise label du formulaire n’est associée à aucun champ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter un attribut for au label</t>
   </si>
 </sst>
 </file>
@@ -419,20 +452,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB78"/>
+  <dimension ref="A1:AB92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E93" activeCellId="0" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="90.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.61"/>
@@ -528,7 +561,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
@@ -537,19 +570,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -558,19 +591,19 @@
         <v>5</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>9</v>
@@ -579,19 +612,19 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
@@ -600,19 +633,19 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
@@ -621,19 +654,19 @@
         <v>8</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>13</v>
@@ -642,19 +675,19 @@
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>9</v>
@@ -663,19 +696,19 @@
         <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>13</v>
@@ -684,61 +717,61 @@
         <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>9</v>
@@ -747,19 +780,19 @@
         <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>9</v>
@@ -768,19 +801,19 @@
         <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
@@ -789,19 +822,19 @@
         <v>74</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
@@ -810,19 +843,19 @@
         <v>83</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>9</v>
@@ -831,19 +864,19 @@
         <v>136</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>9</v>
@@ -852,19 +885,19 @@
         <v>153</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>9</v>
@@ -873,19 +906,19 @@
         <v>205</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>9</v>
@@ -894,19 +927,19 @@
         <v>220</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>13</v>
@@ -915,19 +948,19 @@
         <v>34</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>13</v>
@@ -936,19 +969,19 @@
         <v>61</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>13</v>
@@ -957,19 +990,19 @@
         <v>79</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>13</v>
@@ -978,19 +1011,19 @@
         <v>83</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>13</v>
@@ -999,19 +1032,19 @@
         <v>100</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>13</v>
@@ -1020,19 +1053,19 @@
         <v>128</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>9</v>
@@ -1053,7 +1086,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>9</v>
@@ -1074,7 +1107,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>9</v>
@@ -1095,7 +1128,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>9</v>
@@ -1116,7 +1149,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>9</v>
@@ -1137,7 +1170,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>9</v>
@@ -1158,7 +1191,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>9</v>
@@ -1179,7 +1212,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>9</v>
@@ -1200,7 +1233,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>9</v>
@@ -1221,7 +1254,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>9</v>
@@ -1242,7 +1275,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>9</v>
@@ -1263,7 +1296,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>9</v>
@@ -1284,7 +1317,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>13</v>
@@ -1305,7 +1338,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>9</v>
@@ -1326,7 +1359,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>9</v>
@@ -1347,7 +1380,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>9</v>
@@ -1368,7 +1401,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>9</v>
@@ -1389,7 +1422,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>9</v>
@@ -1410,7 +1443,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>13</v>
@@ -2031,7 +2064,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>9</v>
@@ -2051,7 +2084,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>9</v>
@@ -2067,6 +2100,286 @@
       </c>
       <c r="F78" s="0" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour de l'audit SEO
Mise à jour de l'audit SEO
</commit_message>
<xml_diff>
--- a/ressources/Modèle-audit-SEO.xlsx
+++ b/ressources/Modèle-audit-SEO.xlsx
@@ -454,8 +454,8 @@
   </sheetPr>
   <dimension ref="A1:AB92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E93" activeCellId="0" sqref="E93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,8 +464,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="80.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.61"/>
@@ -536,7 +536,9 @@
       <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -704,7 +706,9 @@
       <c r="F10" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -746,7 +750,9 @@
       <c r="F12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -788,7 +794,9 @@
       <c r="F14" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1082,7 +1090,9 @@
       <c r="F28" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -1145,7 +1155,9 @@
       <c r="F31" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1521,6 +1533,9 @@
       <c r="F49" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="G49" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -1960,6 +1975,9 @@
       </c>
       <c r="F71" s="0" t="s">
         <v>60</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,6 +2299,9 @@
       <c r="F87" s="0" t="s">
         <v>70</v>
       </c>
+      <c r="G87" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
@@ -2320,6 +2341,9 @@
       </c>
       <c r="F89" s="0" t="s">
         <v>74</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>